<commit_message>
Testing and Commenting code
</commit_message>
<xml_diff>
--- a/Documents/Time_recording.xlsx
+++ b/Documents/Time_recording.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="142">
   <si>
     <t>Nr</t>
   </si>
@@ -447,6 +447,15 @@
   </si>
   <si>
     <t>Searched for error which would kill the app</t>
+  </si>
+  <si>
+    <t>Testing and documenting</t>
+  </si>
+  <si>
+    <t>Documenting and testing the code</t>
+  </si>
+  <si>
+    <t>Design an icon</t>
   </si>
 </sst>
 </file>
@@ -2841,7 +2850,7 @@
       </c>
       <c r="AF13" s="92">
         <f>AD14-AE13</f>
-        <v>-31</v>
+        <v>-24</v>
       </c>
     </row>
     <row r="14" spans="2:33" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -2901,7 +2910,7 @@
       </c>
       <c r="U14" s="32">
         <f>'Std-A'!$C$133</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="V14" s="32">
         <f>'Std-A'!$C$144</f>
@@ -2937,7 +2946,7 @@
       </c>
       <c r="AD14" s="33">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="AE14" s="87"/>
       <c r="AF14" s="89"/>
@@ -2999,7 +3008,7 @@
       </c>
       <c r="U15" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="V15" s="29">
         <f t="shared" ref="V15:AC15" si="2">V14-V13</f>
@@ -3035,7 +3044,7 @@
       </c>
       <c r="AD15" s="30">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="AE15" s="91"/>
       <c r="AF15" s="94"/>
@@ -4935,8 +4944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="45" zoomScaleNormal="45" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H131" sqref="H131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6487,23 +6496,35 @@
       <c r="A127" s="71">
         <v>1</v>
       </c>
-      <c r="B127" s="72"/>
-      <c r="C127" s="73"/>
+      <c r="B127" s="81" t="s">
+        <v>139</v>
+      </c>
+      <c r="C127" s="73">
+        <v>320</v>
+      </c>
       <c r="D127" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="E127" s="72"/>
+      <c r="E127" s="81" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="128" spans="1:5" s="74" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="71">
         <v>2</v>
       </c>
-      <c r="B128" s="72"/>
-      <c r="C128" s="73"/>
+      <c r="B128" s="81" t="s">
+        <v>141</v>
+      </c>
+      <c r="C128" s="73">
+        <v>80</v>
+      </c>
       <c r="D128" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="E128" s="72"/>
+      <c r="E128" s="81" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="129" spans="1:5" s="74" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="71">
@@ -6556,7 +6577,7 @@
       <c r="B133" s="187"/>
       <c r="C133" s="78">
         <f>ROUND((SUM(C127:C132)/60),0)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D133" s="182" t="s">
         <v>18</v>

</xml_diff>